<commit_message>
Fix Product import Friendly name
</commit_message>
<xml_diff>
--- a/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
+++ b/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ProductDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="76">
   <si>
     <t xml:space="preserve">ProductID</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">Sku</t>
   </si>
   <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">BrandName</t>
   </si>
   <si>
@@ -50,12 +53,6 @@
     <t xml:space="preserve">ProductDetails</t>
   </si>
   <si>
-    <t xml:space="preserve">TreatmentInformation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DosageInstructions</t>
-  </si>
-  <si>
     <t xml:space="preserve">FriendlyPageName</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
     <t xml:space="preserve">Hair Care</t>
   </si>
   <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Himalaya</t>
   </si>
   <si>
@@ -113,6 +113,9 @@
     <t xml:space="preserve">Hair Oils</t>
   </si>
   <si>
+    <t xml:space="preserve">test2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Axcer</t>
   </si>
   <si>
@@ -126,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cervical Pillow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3</t>
   </si>
   <si>
     <t xml:space="preserve">image2.png</t>
@@ -252,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -311,12 +317,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -370,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -411,11 +411,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,11 +419,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,10 +506,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,21 +517,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="19" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="18" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,41 +587,38 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="54.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>123</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="G2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>23</v>
@@ -636,41 +627,38 @@
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="O2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="4" t="n">
+      <c r="P2" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="Q2" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="R2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="54.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
@@ -686,14 +674,14 @@
       <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="n">
         <v>300</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>23</v>
@@ -702,46 +690,43 @@
         <v>23</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="M3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="O3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="4" t="n">
+      <c r="P3" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="Q3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="R3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-    </row>
-    <row r="4" s="8" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" s="8" customFormat="true" ht="54.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>29</v>
@@ -749,15 +734,15 @@
       <c r="D4" s="6" t="n">
         <v>125</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6" t="n">
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>23</v>
@@ -766,44 +751,42 @@
         <v>23</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="M4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="6" t="n">
+      <c r="P4" s="6" t="n">
         <v>5</v>
       </c>
+      <c r="Q4" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="R4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="P2:P4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="O2:O4" type="list">
       <formula1>"Percentage,Fixed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -825,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E2:E4 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -839,55 +822,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,19 +878,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="11" t="s">
         <v>59</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="M2" s="9" t="n">
         <v>200</v>
@@ -933,19 +916,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>250</v>
@@ -971,19 +954,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>300</v>
@@ -1009,13 +992,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>75</v>
@@ -1041,13 +1024,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>100</v>
@@ -1073,13 +1056,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M7" s="9" t="n">
         <v>150</v>
@@ -1105,12 +1088,12 @@
         <v>2</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="12" t="n">
+        <v>70</v>
+      </c>
+      <c r="D8" s="11" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="9" t="n">
@@ -1137,12 +1120,12 @@
         <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="13" t="n">
+        <v>70</v>
+      </c>
+      <c r="D9" s="12" t="n">
         <v>2</v>
       </c>
       <c r="M9" s="9" t="n">
@@ -1169,12 +1152,12 @@
         <v>2</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="13" t="n">
+        <v>70</v>
+      </c>
+      <c r="D10" s="12" t="n">
         <v>3</v>
       </c>
       <c r="M10" s="9" t="n">
@@ -1201,30 +1184,30 @@
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="13" t="n">
+        <v>72</v>
+      </c>
+      <c r="D11" s="12" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M11" s="14" t="n">
+        <v>74</v>
+      </c>
+      <c r="M11" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="N11" s="14" t="n">
+      <c r="N11" s="13" t="n">
         <v>85</v>
       </c>
-      <c r="O11" s="14" t="n">
+      <c r="O11" s="13" t="n">
         <v>110</v>
       </c>
-      <c r="P11" s="14" t="n">
+      <c r="P11" s="13" t="n">
         <v>415</v>
       </c>
       <c r="Q11" s="9" t="n">
@@ -1239,30 +1222,30 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="13" t="n">
+        <v>72</v>
+      </c>
+      <c r="D12" s="12" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="14" t="n">
+        <v>75</v>
+      </c>
+      <c r="M12" s="13" t="n">
         <v>110</v>
       </c>
-      <c r="N12" s="14" t="n">
+      <c r="N12" s="13" t="n">
         <v>90</v>
       </c>
-      <c r="O12" s="14" t="n">
+      <c r="O12" s="13" t="n">
         <v>125</v>
       </c>
-      <c r="P12" s="14" t="n">
+      <c r="P12" s="13" t="n">
         <v>600</v>
       </c>
       <c r="Q12" s="9" t="n">
@@ -1277,30 +1260,30 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="13" t="n">
+        <v>72</v>
+      </c>
+      <c r="D13" s="12" t="n">
         <v>3</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M13" s="14" t="n">
+        <v>74</v>
+      </c>
+      <c r="M13" s="13" t="n">
         <v>120</v>
       </c>
-      <c r="N13" s="14" t="n">
+      <c r="N13" s="13" t="n">
         <v>95</v>
       </c>
-      <c r="O13" s="14" t="n">
+      <c r="O13" s="13" t="n">
         <v>140</v>
       </c>
-      <c r="P13" s="14" t="n">
+      <c r="P13" s="13" t="n">
         <v>1000</v>
       </c>
       <c r="Q13" s="9" t="n">

</xml_diff>

<commit_message>
Remove Dosage instruction Column in Import Sheet
</commit_message>
<xml_diff>
--- a/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
+++ b/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
@@ -509,7 +509,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2:E4"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -809,7 +809,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E2:E4 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Delete sku column in product sheet
</commit_message>
<xml_diff>
--- a/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
+++ b/public/theme/sample_datas/PacificMediHub Import Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ProductDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t xml:space="preserve">ProductID</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t xml:space="preserve">CategoryName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sku</t>
   </si>
   <si>
     <t xml:space="preserve">BrandName</t>
@@ -527,10 +524,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="1" sqref="A11:A13 A5"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -538,19 +535,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="17" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="16" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,201 +599,190 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>123</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="L2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="4" t="n">
+      <c r="N2" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="O2" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="P2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="n">
-        <v>124</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="4" t="n">
+        <v>300</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <v>300</v>
-      </c>
       <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="N3" s="4" t="n">
         <v>5</v>
       </c>
+      <c r="O3" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="P3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
     </row>
     <row r="4" s="9" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>125</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="7" t="n">
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="7" t="n">
-        <v>5</v>
+      <c r="O4" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
+      <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="N2:N4" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="M2:M4" type="list">
       <formula1>"Percentage,Fixed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -818,8 +804,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A11:A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -832,55 +818,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,25 +874,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="M2" s="10" t="n">
         <v>200</v>
@@ -924,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,25 +918,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="D3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="M3" s="10" t="n">
         <v>250</v>
@@ -968,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,25 +962,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="D4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="M4" s="10" t="n">
         <v>300</v>
@@ -1012,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,13 +1006,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="M5" s="10" t="n">
         <v>75</v>
@@ -1044,7 +1030,7 @@
         <v>2</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,13 +1038,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M6" s="10" t="n">
         <v>100</v>
@@ -1076,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,13 +1070,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M7" s="10" t="n">
         <v>150</v>
@@ -1108,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,10 +1102,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="14" t="n">
         <v>1</v>
@@ -1140,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,10 +1134,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>2</v>
@@ -1172,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1180,10 +1166,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>3</v>
@@ -1204,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,19 +1198,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="M11" s="16" t="n">
         <v>100</v>
@@ -1242,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="R11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,19 +1236,19 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M12" s="16" t="n">
         <v>110</v>
@@ -1280,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,19 +1274,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>3</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="M13" s="16" t="n">
         <v>120</v>
@@ -1318,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>